<commit_message>
Updated using data downloads on 2021-09-27 (EDT).
</commit_message>
<xml_diff>
--- a/israel_covid.xlsx
+++ b/israel_covid.xlsx
@@ -431,22 +431,22 @@
         <v>12-15</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>581</v>
+        <v>383</v>
       </c>
       <c r="D3">
-        <v>4986</v>
+        <v>3727</v>
       </c>
       <c r="E3">
-        <v>581.4</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>239.1</v>
+        <v>130.3</v>
       </c>
       <c r="G3">
-        <v>1686.4</v>
+        <v>1361.5</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -472,22 +472,22 @@
         <v>16-19</v>
       </c>
       <c r="B4">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C4">
-        <v>3575</v>
+        <v>1536</v>
       </c>
       <c r="D4">
-        <v>2091</v>
+        <v>1509</v>
       </c>
       <c r="E4">
-        <v>73.3</v>
+        <v>58.9</v>
       </c>
       <c r="F4">
-        <v>960</v>
+        <v>519.8</v>
       </c>
       <c r="G4">
-        <v>1437</v>
+        <v>1086.2</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -505,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="5">
@@ -513,28 +513,28 @@
         <v>20-29</v>
       </c>
       <c r="B5">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="C5">
-        <v>9087</v>
+        <v>4091</v>
       </c>
       <c r="D5">
-        <v>3475</v>
+        <v>2783</v>
       </c>
       <c r="E5">
-        <v>135.6</v>
+        <v>64.1</v>
       </c>
       <c r="F5">
-        <v>1061.4</v>
+        <v>629.2</v>
       </c>
       <c r="G5">
-        <v>1316.6</v>
+        <v>1105.3</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <v>14</v>
@@ -543,10 +543,10 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="M5">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="6">
@@ -554,40 +554,40 @@
         <v>30-39</v>
       </c>
       <c r="B6">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="C6">
-        <v>7986</v>
+        <v>4499</v>
       </c>
       <c r="D6">
-        <v>3128</v>
+        <v>2797</v>
       </c>
       <c r="E6">
-        <v>193.5</v>
+        <v>118.7</v>
       </c>
       <c r="F6">
-        <v>1115.6</v>
+        <v>804.5</v>
       </c>
       <c r="G6">
-        <v>1644.9</v>
+        <v>1543.6</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>13.7</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="7">
@@ -595,40 +595,40 @@
         <v>40-49</v>
       </c>
       <c r="B7">
-        <v>781</v>
+        <v>511</v>
       </c>
       <c r="C7">
-        <v>5316</v>
+        <v>2729</v>
       </c>
       <c r="D7">
-        <v>2191</v>
+        <v>1952</v>
       </c>
       <c r="E7">
-        <v>194.1</v>
+        <v>96.5</v>
       </c>
       <c r="F7">
-        <v>998.6</v>
+        <v>661.7</v>
       </c>
       <c r="G7">
-        <v>1502.5</v>
+        <v>1401.3</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="K7">
-        <v>1.7</v>
+        <v>0.4</v>
       </c>
       <c r="L7">
-        <v>2.3</v>
+        <v>2.7</v>
       </c>
       <c r="M7">
-        <v>46.6</v>
+        <v>59.6</v>
       </c>
     </row>
     <row r="8">
@@ -636,40 +636,40 @@
         <v>50-59</v>
       </c>
       <c r="B8">
-        <v>544</v>
+        <v>309</v>
       </c>
       <c r="C8">
-        <v>2369</v>
+        <v>1189</v>
       </c>
       <c r="D8">
-        <v>1169</v>
+        <v>1047</v>
       </c>
       <c r="E8">
-        <v>123.7</v>
+        <v>61.4</v>
       </c>
       <c r="F8">
-        <v>751</v>
+        <v>461.6</v>
       </c>
       <c r="G8">
-        <v>1165.1</v>
+        <v>1098.9</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J8">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="K8">
-        <v>1.1</v>
+        <v>0.8</v>
       </c>
       <c r="L8">
-        <v>10.8</v>
+        <v>7.8</v>
       </c>
       <c r="M8">
-        <v>69.8</v>
+        <v>110.2</v>
       </c>
     </row>
     <row r="9">
@@ -677,40 +677,40 @@
         <v>60-69</v>
       </c>
       <c r="B9">
-        <v>464</v>
+        <v>281</v>
       </c>
       <c r="C9">
-        <v>1155</v>
+        <v>708</v>
       </c>
       <c r="D9">
-        <v>756</v>
+        <v>669</v>
       </c>
       <c r="E9">
-        <v>92.8</v>
+        <v>53.2</v>
       </c>
       <c r="F9">
-        <v>684.8</v>
+        <v>494.6</v>
       </c>
       <c r="G9">
-        <v>1120.8</v>
+        <v>1023.2</v>
       </c>
       <c r="H9">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I9">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J9">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K9">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="L9">
-        <v>22.5</v>
+        <v>23.8</v>
       </c>
       <c r="M9">
-        <v>161.6</v>
+        <v>159.1</v>
       </c>
     </row>
     <row r="10">
@@ -718,40 +718,40 @@
         <v>70-79</v>
       </c>
       <c r="B10">
-        <v>347</v>
+        <v>211</v>
       </c>
       <c r="C10">
-        <v>590</v>
+        <v>330</v>
       </c>
       <c r="D10">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E10">
-        <v>89.6</v>
+        <v>52.4</v>
       </c>
       <c r="F10">
-        <v>689</v>
+        <v>450.1</v>
       </c>
       <c r="G10">
-        <v>775.9</v>
+        <v>822.6</v>
       </c>
       <c r="H10">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I10">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="J10">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K10">
-        <v>4.6</v>
+        <v>4</v>
       </c>
       <c r="L10">
-        <v>59.6</v>
+        <v>36.8</v>
       </c>
       <c r="M10">
-        <v>135.6</v>
+        <v>177.8</v>
       </c>
     </row>
     <row r="11">
@@ -759,40 +759,40 @@
         <v>80-89</v>
       </c>
       <c r="B11">
-        <v>259</v>
+        <v>136</v>
       </c>
       <c r="C11">
-        <v>377</v>
+        <v>206</v>
       </c>
       <c r="D11">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="E11">
-        <v>153.6</v>
+        <v>77.6</v>
       </c>
       <c r="F11">
-        <v>871.2</v>
+        <v>543.3</v>
       </c>
       <c r="G11">
-        <v>1051.3</v>
+        <v>976.5</v>
       </c>
       <c r="H11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I11">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J11">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K11">
-        <v>13</v>
+        <v>6.8</v>
       </c>
       <c r="L11">
-        <v>76.3</v>
+        <v>52.7</v>
       </c>
       <c r="M11">
-        <v>148.9</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12">
@@ -800,40 +800,40 @@
         <v>90+</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C12">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="D12">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E12">
-        <v>224.7</v>
+        <v>171.4</v>
       </c>
       <c r="F12">
-        <v>798</v>
+        <v>449.6</v>
       </c>
       <c r="G12">
-        <v>776.9</v>
+        <v>931.1</v>
       </c>
       <c r="H12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J12">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12">
-        <v>20.7</v>
+        <v>14</v>
       </c>
       <c r="L12">
-        <v>42.4</v>
+        <v>38.8</v>
       </c>
       <c r="M12">
-        <v>213.9</v>
+        <v>214.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated using data downloaded on 2021-09-29.
</commit_message>
<xml_diff>
--- a/israel_covid.xlsx
+++ b/israel_covid.xlsx
@@ -434,19 +434,19 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>383</v>
+        <v>329</v>
       </c>
       <c r="D3">
-        <v>3727</v>
+        <v>3162</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>130.3</v>
+        <v>110.2</v>
       </c>
       <c r="G3">
-        <v>1361.5</v>
+        <v>1169.1</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -472,22 +472,22 @@
         <v>16-19</v>
       </c>
       <c r="B4">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C4">
-        <v>1536</v>
+        <v>1317</v>
       </c>
       <c r="D4">
-        <v>1509</v>
+        <v>1345</v>
       </c>
       <c r="E4">
-        <v>58.9</v>
+        <v>50.3</v>
       </c>
       <c r="F4">
-        <v>519.8</v>
+        <v>447.4</v>
       </c>
       <c r="G4">
-        <v>1086.2</v>
+        <v>978.8</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -505,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5">
@@ -513,28 +513,28 @@
         <v>20-29</v>
       </c>
       <c r="B5">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="C5">
-        <v>4091</v>
+        <v>3483</v>
       </c>
       <c r="D5">
-        <v>2783</v>
+        <v>2478</v>
       </c>
       <c r="E5">
-        <v>64.1</v>
+        <v>51.5</v>
       </c>
       <c r="F5">
-        <v>629.2</v>
+        <v>540.8</v>
       </c>
       <c r="G5">
-        <v>1105.3</v>
+        <v>993.2</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>14</v>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="M5">
         <v>5.6</v>
@@ -554,40 +554,40 @@
         <v>30-39</v>
       </c>
       <c r="B6">
-        <v>507</v>
+        <v>447</v>
       </c>
       <c r="C6">
-        <v>4499</v>
+        <v>3684</v>
       </c>
       <c r="D6">
-        <v>2797</v>
+        <v>2495</v>
       </c>
       <c r="E6">
-        <v>118.7</v>
+        <v>103</v>
       </c>
       <c r="F6">
-        <v>804.5</v>
+        <v>665.6</v>
       </c>
       <c r="G6">
-        <v>1543.6</v>
+        <v>1392</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="M6">
-        <v>19.3</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="7">
@@ -595,40 +595,40 @@
         <v>40-49</v>
       </c>
       <c r="B7">
-        <v>511</v>
+        <v>468</v>
       </c>
       <c r="C7">
-        <v>2729</v>
+        <v>2379</v>
       </c>
       <c r="D7">
-        <v>1952</v>
+        <v>1737</v>
       </c>
       <c r="E7">
-        <v>96.5</v>
+        <v>87.5</v>
       </c>
       <c r="F7">
-        <v>661.7</v>
+        <v>583</v>
       </c>
       <c r="G7">
-        <v>1401.3</v>
+        <v>1260.2</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J7">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="K7">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="L7">
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="M7">
-        <v>59.6</v>
+        <v>50.1</v>
       </c>
     </row>
     <row r="8">
@@ -636,40 +636,40 @@
         <v>50-59</v>
       </c>
       <c r="B8">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="C8">
-        <v>1189</v>
+        <v>1015</v>
       </c>
       <c r="D8">
-        <v>1047</v>
+        <v>1017</v>
       </c>
       <c r="E8">
-        <v>61.4</v>
+        <v>54.1</v>
       </c>
       <c r="F8">
-        <v>461.6</v>
+        <v>398.1</v>
       </c>
       <c r="G8">
-        <v>1098.9</v>
+        <v>1079.8</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J8">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K8">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="L8">
-        <v>7.8</v>
+        <v>6.7</v>
       </c>
       <c r="M8">
-        <v>110.2</v>
+        <v>116.8</v>
       </c>
     </row>
     <row r="9">
@@ -677,28 +677,28 @@
         <v>60-69</v>
       </c>
       <c r="B9">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="C9">
-        <v>708</v>
+        <v>638</v>
       </c>
       <c r="D9">
-        <v>669</v>
+        <v>626</v>
       </c>
       <c r="E9">
-        <v>53.2</v>
+        <v>49.6</v>
       </c>
       <c r="F9">
-        <v>494.6</v>
+        <v>450.6</v>
       </c>
       <c r="G9">
-        <v>1023.2</v>
+        <v>964.7</v>
       </c>
       <c r="H9">
         <v>11</v>
       </c>
       <c r="I9">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J9">
         <v>104</v>
@@ -707,10 +707,10 @@
         <v>2.1</v>
       </c>
       <c r="L9">
-        <v>23.8</v>
+        <v>22.6</v>
       </c>
       <c r="M9">
-        <v>159.1</v>
+        <v>160.3</v>
       </c>
     </row>
     <row r="10">
@@ -718,40 +718,40 @@
         <v>70-79</v>
       </c>
       <c r="B10">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C10">
-        <v>330</v>
+        <v>297</v>
       </c>
       <c r="D10">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="E10">
-        <v>52.4</v>
+        <v>49.2</v>
       </c>
       <c r="F10">
-        <v>450.1</v>
+        <v>409.9</v>
       </c>
       <c r="G10">
-        <v>822.6</v>
+        <v>786.3</v>
       </c>
       <c r="H10">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I10">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J10">
         <v>80</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="L10">
-        <v>36.8</v>
+        <v>40</v>
       </c>
       <c r="M10">
-        <v>177.8</v>
+        <v>179.2</v>
       </c>
     </row>
     <row r="11">
@@ -759,40 +759,40 @@
         <v>80-89</v>
       </c>
       <c r="B11">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C11">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D11">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E11">
-        <v>77.6</v>
+        <v>74</v>
       </c>
       <c r="F11">
-        <v>543.3</v>
+        <v>554.5</v>
       </c>
       <c r="G11">
-        <v>976.5</v>
+        <v>978.1</v>
       </c>
       <c r="H11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J11">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K11">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="L11">
-        <v>52.7</v>
+        <v>61.3</v>
       </c>
       <c r="M11">
-        <v>175</v>
+        <v>190.1</v>
       </c>
     </row>
     <row r="12">
@@ -800,40 +800,40 @@
         <v>90+</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C12">
         <v>58</v>
       </c>
       <c r="D12">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E12">
-        <v>171.4</v>
+        <v>151.1</v>
       </c>
       <c r="F12">
-        <v>449.6</v>
+        <v>453</v>
       </c>
       <c r="G12">
-        <v>931.1</v>
+        <v>805.4</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J12">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="K12">
-        <v>14</v>
+        <v>2.8</v>
       </c>
       <c r="L12">
-        <v>38.8</v>
+        <v>31.2</v>
       </c>
       <c r="M12">
-        <v>214.9</v>
+        <v>156.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for data as of 2021-10-13.
- Note that there are no severe illness cases among 90+ without booster, so numbers are weird there.
</commit_message>
<xml_diff>
--- a/israel_covid.xlsx
+++ b/israel_covid.xlsx
@@ -390,37 +390,37 @@
         <v>קבוצת גיל</v>
       </c>
       <c r="B2" t="str">
-        <v>חולים פעילים מחוסנים עם דחף</v>
+        <v>חולים פעילים מחוסנים</v>
       </c>
       <c r="C2" t="str">
-        <v>חולים פעילים מחוסנים ללא דחף</v>
+        <v>חולים פעילים מחוסנים ללא תוקף</v>
       </c>
       <c r="D2" t="str">
         <v>חולים פעילים לא מחוסנים</v>
       </c>
       <c r="E2" t="str">
-        <v>חולים פעילים מחוסנים עם דחף ל-100 אלף תושבים</v>
+        <v>חולים פעילים מחוסנים ל-100 אלף תושבים</v>
       </c>
       <c r="F2" t="str">
-        <v>חולים פעילים מחוסנים ללא דחף ל-100 אלף תושבים</v>
+        <v>חולים פעילים מחוסנים ללא תוקף ל-100 אלף תושבים</v>
       </c>
       <c r="G2" t="str">
         <v xml:space="preserve">חולים פעילים לא מחוסנים ל-100 אלף תושבים </v>
       </c>
       <c r="H2" t="str">
-        <v>חולים קשה מחוסנים עם דחף</v>
+        <v>חולים קשה מחוסנים</v>
       </c>
       <c r="I2" t="str">
-        <v>חולים קשה מחוסנים ללא דחף</v>
+        <v>חולים קשה מחוסנים ללא תוקף</v>
       </c>
       <c r="J2" t="str">
         <v>חולים קשה לא מחוסנים</v>
       </c>
       <c r="K2" t="str">
-        <v>חולים קשה מחוסנים עם דחף ל-100 אלף תושבים</v>
+        <v>חולים קשה מחוסנים ל-100 אלף תושבים</v>
       </c>
       <c r="L2" t="str">
-        <v>חולים קשה מחוסנים ללא דחף ל-100 אלף תושבים</v>
+        <v>חולים קשה מחוסנים ללא תוקף ל-100 אלף תושבים</v>
       </c>
       <c r="M2" t="str">
         <v>חולים קשה לא מחוסנים ל-100 אלף תושבים</v>
@@ -431,22 +431,22 @@
         <v>12-15</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="C3">
-        <v>329</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3162</v>
+        <v>1411</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>50.6</v>
       </c>
       <c r="F3">
-        <v>110.2</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1169.1</v>
+        <v>550.8</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4">
@@ -472,22 +472,22 @@
         <v>16-19</v>
       </c>
       <c r="B4">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="C4">
-        <v>1317</v>
+        <v>291</v>
       </c>
       <c r="D4">
-        <v>1345</v>
+        <v>684</v>
       </c>
       <c r="E4">
-        <v>50.3</v>
+        <v>58.9</v>
       </c>
       <c r="F4">
-        <v>447.4</v>
+        <v>289.4</v>
       </c>
       <c r="G4">
-        <v>978.8</v>
+        <v>536.5</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -505,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5">
@@ -513,40 +513,40 @@
         <v>20-29</v>
       </c>
       <c r="B5">
-        <v>194</v>
+        <v>481</v>
       </c>
       <c r="C5">
-        <v>3483</v>
+        <v>774</v>
       </c>
       <c r="D5">
-        <v>2478</v>
+        <v>1239</v>
       </c>
       <c r="E5">
-        <v>51.5</v>
+        <v>63.5</v>
       </c>
       <c r="F5">
-        <v>540.8</v>
+        <v>304.5</v>
       </c>
       <c r="G5">
-        <v>993.2</v>
+        <v>544.5</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L5">
-        <v>0.3</v>
+        <v>1.2</v>
       </c>
       <c r="M5">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="6">
@@ -554,22 +554,22 @@
         <v>30-39</v>
       </c>
       <c r="B6">
-        <v>447</v>
+        <v>511</v>
       </c>
       <c r="C6">
-        <v>3684</v>
+        <v>846</v>
       </c>
       <c r="D6">
-        <v>2495</v>
+        <v>1210</v>
       </c>
       <c r="E6">
-        <v>103</v>
+        <v>67.6</v>
       </c>
       <c r="F6">
-        <v>665.6</v>
+        <v>374.5</v>
       </c>
       <c r="G6">
-        <v>1392</v>
+        <v>739.3</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -578,16 +578,16 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="M6">
-        <v>16.7</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="7">
@@ -595,40 +595,40 @@
         <v>40-49</v>
       </c>
       <c r="B7">
-        <v>468</v>
+        <v>384</v>
       </c>
       <c r="C7">
-        <v>2379</v>
+        <v>576</v>
       </c>
       <c r="D7">
-        <v>1737</v>
+        <v>843</v>
       </c>
       <c r="E7">
-        <v>87.5</v>
+        <v>49.2</v>
       </c>
       <c r="F7">
-        <v>583</v>
+        <v>356.6</v>
       </c>
       <c r="G7">
-        <v>1260.2</v>
+        <v>669.6</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="K7">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="L7">
-        <v>3.4</v>
+        <v>1.2</v>
       </c>
       <c r="M7">
-        <v>50.1</v>
+        <v>37.3</v>
       </c>
     </row>
     <row r="8">
@@ -636,40 +636,40 @@
         <v>50-59</v>
       </c>
       <c r="B8">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="C8">
-        <v>1015</v>
+        <v>319</v>
       </c>
       <c r="D8">
-        <v>1017</v>
+        <v>518</v>
       </c>
       <c r="E8">
-        <v>54.1</v>
+        <v>34.9</v>
       </c>
       <c r="F8">
-        <v>398.1</v>
+        <v>318.3</v>
       </c>
       <c r="G8">
-        <v>1079.8</v>
+        <v>598.3</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I8">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="J8">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="K8">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="L8">
-        <v>6.7</v>
+        <v>9</v>
       </c>
       <c r="M8">
-        <v>116.8</v>
+        <v>80.8</v>
       </c>
     </row>
     <row r="9">
@@ -677,40 +677,40 @@
         <v>60-69</v>
       </c>
       <c r="B9">
-        <v>263</v>
+        <v>209</v>
       </c>
       <c r="C9">
-        <v>638</v>
+        <v>174</v>
       </c>
       <c r="D9">
-        <v>626</v>
+        <v>337</v>
       </c>
       <c r="E9">
-        <v>49.6</v>
+        <v>33.8</v>
       </c>
       <c r="F9">
-        <v>450.6</v>
+        <v>320.1</v>
       </c>
       <c r="G9">
-        <v>964.7</v>
+        <v>549.3</v>
       </c>
       <c r="H9">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I9">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="J9">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="K9">
-        <v>2.1</v>
+        <v>2.9</v>
       </c>
       <c r="L9">
-        <v>22.6</v>
+        <v>18.4</v>
       </c>
       <c r="M9">
-        <v>160.3</v>
+        <v>101.1</v>
       </c>
     </row>
     <row r="10">
@@ -718,40 +718,40 @@
         <v>70-79</v>
       </c>
       <c r="B10">
-        <v>199</v>
+        <v>157</v>
       </c>
       <c r="C10">
-        <v>297</v>
+        <v>93</v>
       </c>
       <c r="D10">
-        <v>351</v>
+        <v>230</v>
       </c>
       <c r="E10">
-        <v>49.2</v>
+        <v>34.9</v>
       </c>
       <c r="F10">
-        <v>409.9</v>
+        <v>318</v>
       </c>
       <c r="G10">
-        <v>786.3</v>
+        <v>548.8</v>
       </c>
       <c r="H10">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I10">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="J10">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="K10">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="L10">
-        <v>40</v>
+        <v>30.8</v>
       </c>
       <c r="M10">
-        <v>179.2</v>
+        <v>112.1</v>
       </c>
     </row>
     <row r="11">
@@ -759,40 +759,40 @@
         <v>80-89</v>
       </c>
       <c r="B11">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C11">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="D11">
-        <v>211</v>
+        <v>128</v>
       </c>
       <c r="E11">
-        <v>74</v>
+        <v>55.6</v>
       </c>
       <c r="F11">
-        <v>554.5</v>
+        <v>260.9</v>
       </c>
       <c r="G11">
-        <v>978.1</v>
+        <v>626.4</v>
       </c>
       <c r="H11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
         <v>23</v>
       </c>
-      <c r="J11">
-        <v>41</v>
-      </c>
       <c r="K11">
-        <v>6.3</v>
+        <v>5.1</v>
       </c>
       <c r="L11">
-        <v>61.3</v>
+        <v>22.2</v>
       </c>
       <c r="M11">
-        <v>190.1</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="12">
@@ -800,40 +800,40 @@
         <v>90+</v>
       </c>
       <c r="B12">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C12">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D12">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="E12">
-        <v>151.1</v>
+        <v>84.1</v>
       </c>
       <c r="F12">
-        <v>453</v>
+        <v>94.6</v>
       </c>
       <c r="G12">
-        <v>805.4</v>
+        <v>405</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K12">
-        <v>2.8</v>
+        <v>4.8</v>
       </c>
       <c r="L12">
-        <v>31.2</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>156.3</v>
+        <v>126.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>